<commit_message>
resumo estendido COBEM 2019 final
-enviados tension e fiber resumos estendidos.
</commit_message>
<xml_diff>
--- a/Tension/artigo_cobem/imagens/resultados dos modulos de young.xlsx
+++ b/Tension/artigo_cobem/imagens/resultados dos modulos de young.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WORK\programing\Latex\PapersEmAndamento\Tension\artigo_cobem\imagens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6B9BC1-6875-4516-B215-5F16FBB9FE7F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115B371D-AC7D-41F6-8819-679A39F24C45}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="15840" xr2:uid="{1538F110-639C-48EE-BA58-BCA312149310}"/>
   </bookViews>
@@ -206,23 +206,27 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Planilha1!$M$2:$Q$2</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Planilha1!$M$2:$Q$2</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Planilha1!$M$2,Planilha1!$O$2:$Q$2)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>230</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>235</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>240</c:v>
+                  <c:v>245</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>245</c:v>
-                </c:pt>
-                <c:pt idx="4">
                   <c:v>250</c:v>
                 </c:pt>
               </c:numCache>
@@ -230,23 +234,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Planilha1!$C$4,Planilha1!$C$9,Planilha1!$C$14,Planilha1!$C$19,Planilha1!$C$24)</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>(Planilha1!$C$4,Planilha1!$C$9,Planilha1!$C$14,Planilha1!$C$19,Planilha1!$C$24)</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Planilha1!$C$4,Planilha1!$C$14,Planilha1!$C$19,Planilha1!$C$24)</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0.84029200000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.89612199999999986</c:v>
+                  <c:v>0.8542820000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8542820000000001</c:v>
+                  <c:v>0.86101799999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.86101799999999995</c:v>
-                </c:pt>
-                <c:pt idx="4">
                   <c:v>0.89852999999999983</c:v>
                 </c:pt>
               </c:numCache>
@@ -437,7 +445,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -514,7 +522,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1392,7 +1400,7 @@
   <dimension ref="A2:Q28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z30" sqref="Z30"/>
+      <selection activeCell="Z33" sqref="Z33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1653,7 +1661,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="95" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>